<commit_message>
development logic VSM and change stopwords to indonesia
</commit_message>
<xml_diff>
--- a/app/db/databerita.xlsx
+++ b/app/db/databerita.xlsx
@@ -1615,40 +1615,40 @@
     <t>berita  politik</t>
   </si>
   <si>
-    <t>87 anggota polres jombang terima kado tahun baru naik pangkat</t>
-  </si>
-  <si>
-    <t>warga padat balkot surabaya jelang detik ganti tahun</t>
-  </si>
-  <si>
-    <t>kapolda jatim pantau tahun baru rumah dinas batu malang pacet padat</t>
+    <t>87 anggota polres jombang terima kado pangkat</t>
+  </si>
+  <si>
+    <t>warga padat balkot surabaya jelang detik ganti</t>
+  </si>
+  <si>
+    <t>kapolda jatim pantau rumah dinas batu malang pacet padat</t>
   </si>
   <si>
     <t>14 ayam mati panggang gegara sambar petir sleman</t>
   </si>
   <si>
-    <t>tempat hibur ciwidey bandung razia 2 unjung positif sabu</t>
-  </si>
-  <si>
-    <t>jelang tahun baru 2020 samarinda landa 3 peristiwa bakar</t>
-  </si>
-  <si>
-    <t>jelas kemenhub soal sebab banjir tol cipali</t>
-  </si>
-  <si>
-    <t>hamsik tak tarik gabung roma</t>
-  </si>
-  <si>
-    <t>pikap muat melon bakar tewas satu orang tol nganjuk evakuasi</t>
-  </si>
-  <si>
-    <t>raya hut dki usai warga mulai tinggal bundar hi</t>
+    <t>hibur ciwidey bandung razia 2 unjung positif sabu</t>
+  </si>
+  <si>
+    <t>jelang 2020 samarinda landa 3 peristiwa bakar</t>
+  </si>
+  <si>
+    <t>kemenhub banjir tol cipali</t>
+  </si>
+  <si>
+    <t>hamsik tarik gabung as roma</t>
+  </si>
+  <si>
+    <t>pikap muat melon bakar tewas orang tol nganjuk evakuasi</t>
+  </si>
+  <si>
+    <t>raya hut dki warga tinggal bundar hi</t>
   </si>
   <si>
     <t>lionel messi saran istirahat bela timnas argentina</t>
   </si>
   <si>
-    <t>pikap angkut buah bakar tol nganjuk km 662 satu orang tewa</t>
+    <t>pikap angkut buah bakar tol nganjuk km 662 orang tewa</t>
   </si>
   <si>
     <t>upin ipin gedung dprd pacitan</t>
@@ -1657,91 +1657,91 @@
     <t>469 orang ungsi akibat banjir solok selatan sumbar</t>
   </si>
   <si>
-    <t>bwf finals indonesia kirim tiga wakil semifin</t>
+    <t>bwf finals indonesia kirim wakil semifin</t>
   </si>
   <si>
     <t>dwp 2019 ramai tari tradisional panggung utama</t>
   </si>
   <si>
-    <t>sidak rutan makassar tugas temu alat isap hingga timbang narkoba</t>
-  </si>
-  <si>
-    <t>setor pajak 2019 bakal tekor target 2020 nilai terlalu ambisiu</t>
+    <t>sidak rutan makassar tugas temu alat isap timbang narkoba</t>
+  </si>
+  <si>
+    <t>setor pajak 2019 tekor target 2020 nilai ambisiu</t>
   </si>
   <si>
     <t>kobra muncul gunungkidul nyusup kamar bayi bikin warga ngungsi</t>
   </si>
   <si>
-    <t>jokowi ada menteri ekspor mendag wenang presiden</t>
-  </si>
-  <si>
-    <t>pilpres kian dekat tkn minta laku kampanye door door</t>
+    <t>jokowi menteri ekspor mendag wenang presiden</t>
+  </si>
+  <si>
+    <t>pilpres kian tkn laku kampanye door to door</t>
   </si>
   <si>
     <t>keliling pasar ikan modern jokowi standar internasion</t>
   </si>
   <si>
-    <t>kata jacksen barito gagal lolo</t>
-  </si>
-  <si>
-    <t>identitas istri duga teroris nekat ledak diri</t>
+    <t>jacksen barito gagal lolo</t>
+  </si>
+  <si>
+    <t>identitas istri duga teroris nekat ledak</t>
   </si>
   <si>
     <t>proyek talut mangkrak makam karanganyar rawan ambrol</t>
   </si>
   <si>
-    <t>ibu vicky nitinegoro hadir syukur nikita mirzani dapat lampu hijau</t>
-  </si>
-  <si>
-    <t>bpn sindir ruf amin kok tanya pakai sontek</t>
-  </si>
-  <si>
-    <t>ruf janji dana abadi budaya gerindra dana mana</t>
-  </si>
-  <si>
-    <t>edar video salmafina sunan tampak mabuk</t>
-  </si>
-  <si>
-    <t>aksi demo rusuh bandung jumlah orang aman polisi</t>
-  </si>
-  <si>
-    <t>tenang lloris posisi aman kok</t>
-  </si>
-  <si>
-    <t>mobil bakar padam brimobpaskhas jaga depan polsek tn abang</t>
+    <t>vicky nitinegoro hadir syukur nikita mirzani lampu hijau</t>
+  </si>
+  <si>
+    <t>bpn sindir ma ruf amin pakai sontek</t>
+  </si>
+  <si>
+    <t>ma ruf janji dana abadi budaya gerindra dana</t>
+  </si>
+  <si>
+    <t>edar video salmafina sunan mabuk</t>
+  </si>
+  <si>
+    <t>aksi demo rusuh bandung orang aman polisi</t>
+  </si>
+  <si>
+    <t>tenang lloris posisi aman</t>
+  </si>
+  <si>
+    <t>mobil bakar padam brimobpaskhas jaga polsek tn abang</t>
   </si>
   <si>
     <t>dukung 2 partai ratu tatu kantong tiket tuju pilkada serang</t>
   </si>
   <si>
-    <t>faisal basri buka 5 modus korupsi lewat bank bumn</t>
+    <t>faisal basri buka 5 modus korupsi bank bumn</t>
   </si>
   <si>
     <t>bom mobil ledak somalia 78 orang tewa</t>
   </si>
   <si>
-    <t>gempa landa sulawesi tengah sempat ingat tsunami</t>
-  </si>
-  <si>
-    <t>terima kejar jakarta selatan serah plt ketua umum pssi</t>
-  </si>
-  <si>
-    <t>unbk paket c hari pertama 72 serta hadir</t>
-  </si>
-  <si>
-    <t>dampak bangun yia ajar sdn 3 glagah gedung jadi</t>
-  </si>
-  <si>
-    <t>pilih minta aktif tanya c6</t>
-  </si>
-  <si>
-    <t>rawan jojo beri ketrampilan emakemak</t>
+    <t>gempa landa sulawesi tsunami</t>
+  </si>
+  <si>
+    <t>terima kejar jakarta selatan serah plt ketua pssi</t>
+  </si>
+  <si>
+    <t>unbk paket c 72 hadir</t>
+  </si>
+  <si>
+    <t>dampak bangun yia ajar sdn 3 glagah gedung</t>
+  </si>
+  <si>
+    <t>pilih aktif c6</t>
+  </si>
+  <si>
+    <t>rawan jojo ketrampilan emakemak</t>
   </si>
   <si>
     <t>4 caleg tms telanjur cetak surat suara</t>
   </si>
   <si>
-    <t>petrokimia sinergi sama tni ad kawal subsidi pupuk tangan tani</t>
+    <t>petrokimia sinergi tni ad kawal subsidi pupuk tangan tani</t>
   </si>
   <si>
     <t>tampung aspirasi warga pundong piyungan</t>
@@ -1753,7 +1753,7 @@
     <t>jual gas melon ecer pangkal batas 40 persen</t>
   </si>
   <si>
-    <t>24 tahun akper yky cetak generasi awat</t>
+    <t>24 akper yky cetak generasi awat</t>
   </si>
   <si>
     <t>buka praktik awat griya sehat</t>
@@ -1762,16 +1762,16 @@
     <t>rebut hadiah total rp 100 juta drs hm gandung pardiman mm gelar lomba bank sampah sediy</t>
   </si>
   <si>
-    <t>piala presiden 2019 arema ukir sejarah baru</t>
-  </si>
-  <si>
-    <t>jokowi target menang bogor prabowo umum calon menteri</t>
-  </si>
-  <si>
-    <t>siap operasional minimum yia gera penumpangpendaratan pesawat segera diujicoba</t>
-  </si>
-  <si>
-    <t>serta milu imbau turun apk kpu diy siap peta lokasi tp</t>
+    <t>piala presiden 2019 arema ukir sejarah</t>
+  </si>
+  <si>
+    <t>jokowi target menang bogor prabowo calon menteri</t>
+  </si>
+  <si>
+    <t>operasional minimum yia gera penumpangpendaratan pesawat diujicoba</t>
+  </si>
+  <si>
+    <t>milu imbau turun apk kpu diy peta lokasi tp</t>
   </si>
   <si>
     <t>desember dinas budaya diy gelar budaya selasa wagen</t>
@@ -1780,7 +1780,7 @@
     <t>mohammad sofyan st ketua bkm kota tata gusur kunci daya</t>
   </si>
   <si>
-    <t>jelang coblos siap kpu capai 98 persen</t>
+    <t>jelang coblos kpu capai 98 persen</t>
   </si>
   <si>
     <t>milu serentak 2019 sultan hb x nyoblos tps 15 panembahan</t>
@@ -1789,22 +1789,22 @@
     <t>menristek dikti lantik 8 jabat didi achjari ketua lldikti yogyakarta</t>
   </si>
   <si>
-    <t>jelang akhir bayar 1 bpih 88 persen jemaah lunas biaya haji</t>
+    <t>jelang bayar 1 bpih 88 persen jemaah lunas biaya haji</t>
   </si>
   <si>
     <t>sambut nataru ka wisata operasi kereta priority rute jakartajogja</t>
   </si>
   <si>
-    <t>sutanto hartono jogja seperti waterloo bangalor</t>
+    <t>sutanto hartono jogja waterloo bangalor</t>
   </si>
   <si>
     <t>mahasiswa uin jogja tinggal perosok sumur imam salat</t>
   </si>
   <si>
-    <t>lihat dekat bong supit bogem tempat sunat langgan pangeran keraton jogja</t>
-  </si>
-  <si>
-    <t>peluk hangat jogja fashion festival 2020 semua kalang masyarakat</t>
+    <t>lihat bong supit bogem sunat langgan pangeran keraton jogja</t>
+  </si>
+  <si>
+    <t>peluk hangat jogja fashion festival 2020 kalang masyarakat</t>
   </si>
   <si>
     <t>kisah ajar kursus bahasa inggris gratis jogja</t>
@@ -1816,28 +1816,28 @@
     <t>jogja international heritage walk 2019 libat 25 negara</t>
   </si>
   <si>
-    <t>jogja sapa cara istimewa perintah yogyakarta sambut mahasiswa baru</t>
-  </si>
-  <si>
-    <t>gempa guncang banten sekitar asa hingga jawa tengah jogja</t>
-  </si>
-  <si>
-    <t>warnawarni layang hibur serta jogja international kite festival 2019</t>
+    <t>jogja sapa istimewa perintah yogyakarta sambut mahasiswa</t>
+  </si>
+  <si>
+    <t>gempa guncang banten asa jawa jogja</t>
+  </si>
+  <si>
+    <t>warnawarni layang hibur jogja international kite festival 2019</t>
   </si>
   <si>
     <t>seru jalan pasar anak sayang teman jogja</t>
   </si>
   <si>
-    <t>ganti nazar amien rais pemuda asal blora jalan kaki jogja jakarta</t>
-  </si>
-  <si>
-    <t>cicip tolpit hingga bir jawa pasar kangen jogja</t>
+    <t>ganti nazar amien rais pemuda blora jalan kaki jogja jakarta</t>
+  </si>
+  <si>
+    <t>cicip tolpit bir jawa pasar kangen jogja</t>
   </si>
   <si>
     <t>sekolah makam kramat ancam proyek tol solo jogja</t>
   </si>
   <si>
-    <t>perintah siap trans jogja jakartayogyakarta tak perlu keluar masuk tol</t>
+    <t>perintah trans jogja jakartayogyakarta masuk tol</t>
   </si>
   <si>
     <t>warga jogja bangun sahur pesawat tempur tni au potret 3 pilot</t>
@@ -1846,7 +1846,7 @@
     <t>jaring wisman rusia kemenpar kenal jogja b</t>
   </si>
   <si>
-    <t>hebat nenek asal jogja andal dompet digital jual pasar tradision</t>
+    <t>hebat nenek jogja andal dompet digital jual pasar tradision</t>
   </si>
   <si>
     <t>detik cctv mati tim densus 88 tangkap pria jogja</t>
@@ -1855,37 +1855,37 @@
     <t>tpst piyungan tutup jogja darurat sampah</t>
   </si>
   <si>
-    <t>jokowi naik sepeda ontel acara deklarasi alumni jogja</t>
-  </si>
-  <si>
-    <t>reaksi unik gibran rakabuming soal polemik lagu jogja istimewa</t>
-  </si>
-  <si>
-    <t>tak terima jogja istimewa pakai kampanye capres kill dj lapor polisi</t>
-  </si>
-  <si>
-    <t>balik makna lagu jogja istimewa pakai kampanye prabowosandi</t>
-  </si>
-  <si>
-    <t>mulai tahun baru gera jogja bersih sampah</t>
+    <t>jokowi sepeda ontel acara deklarasi alumni jogja</t>
+  </si>
+  <si>
+    <t>reaksi unik gibran rakabuming polemik lagu jogja istimewa</t>
+  </si>
+  <si>
+    <t>terima jogja istimewa pakai kampanye capres kill the dj lapor polisi</t>
+  </si>
+  <si>
+    <t>makna lagu jogja istimewa pakai kampanye prabowosandi</t>
+  </si>
+  <si>
+    <t>gera jogja bersih sampah</t>
   </si>
   <si>
     <t>hujung 2019 lkb nyaba kampus fkip uhamka</t>
   </si>
   <si>
-    <t>kenal aly kampus khusus pesantren bas kitab kun</t>
-  </si>
-  <si>
-    <t>awal tugas kampus frans santoso jadi terjemah bahasa isyarat gereja katedr</t>
+    <t>kenal ma had aly kampus khusus pesantren bas kitab kun</t>
+  </si>
+  <si>
+    <t>tugas kampus frans santoso terjemah bahasa isyarat gereja katedr</t>
   </si>
   <si>
     <t>kampus china hapus hak bebas pikir mahasiswa</t>
   </si>
   <si>
-    <t>265 kampus ikut program magang 110 bumn</t>
-  </si>
-  <si>
-    <t>fakta tinggal mahasiswa jakarta ikut menwa kampu</t>
+    <t>265 kampus program magang 110 bumn</t>
+  </si>
+  <si>
+    <t>fakta tinggal mahasiswa jakarta menwa kampu</t>
   </si>
   <si>
     <t>mahasiswa kampus swasta tinggal keluh sakit latih menwa</t>
@@ -1894,19 +1894,19 @@
     <t>mahasiswa kampus swasta jakarta kabar tinggal latih menwa</t>
   </si>
   <si>
-    <t>ruf amin minta kampus islam redam sebar paham radik</t>
+    <t>ma ruf amin kampus islam redam sebar paham radik</t>
   </si>
   <si>
     <t>pemuda tangkap basah jebol dinding kampus cilegon</t>
   </si>
   <si>
-    <t>sabet anugerah kampus informatif ipb harap jadi contoh universitas indonesia</t>
+    <t>sabet anugerah kampus informatif ipb harap contoh universitas indonesia</t>
   </si>
   <si>
     <t>polisi hong kong temu 4 000 molotov kampus duduk demonstran</t>
   </si>
   <si>
-    <t>demo kampus hong kong mahasiswa indonesia pilih pulang tki tetap tahan</t>
+    <t>demo kampus hong kong mahasiswa indonesia pilih pulang tki tahan</t>
   </si>
   <si>
     <t>drama demonstran hong kong usaha kabur kampus kepung polisi</t>
@@ -1918,16 +1918,16 @@
     <t>ketua mpr ajak dunia kampus aktif bahas amandemen batas uud nri 1945</t>
   </si>
   <si>
-    <t>polisi hong kong akhir kepung kampus 600 demonstran serah diri</t>
-  </si>
-  <si>
-    <t>kerja sama mit bri institute jadi kampus fintech pertama indonesia</t>
-  </si>
-  <si>
-    <t>polisi hong kong kepung kampus lama bentrok demonstrasi baru</t>
-  </si>
-  <si>
-    <t>atas stress kampus ajak mahasiswa tidur liang lahat</t>
+    <t>polisi hong kong kepung kampus 600 demonstran serah</t>
+  </si>
+  <si>
+    <t>kerja mit bri institute kampus fintech indonesia</t>
+  </si>
+  <si>
+    <t>polisi hong kong kepung kampus bentrok demonstrasi</t>
+  </si>
+  <si>
+    <t>stress kampus ajak mahasiswa tidur liang lahat</t>
   </si>
   <si>
     <t>lembaga budaya betawi undang kampus kolaborasi kembang budaya</t>
@@ -1939,25 +1939,25 @@
     <t>mahasiswa umi makassar tewas serang kelompok orang topeng kampu</t>
   </si>
   <si>
-    <t>demo hong kong picu sekolah tutup hingga polisi tembak gas air mata kampu</t>
-  </si>
-  <si>
-    <t>sekolah kampus pusat belanja manila tutup lama sea games 2019</t>
-  </si>
-  <si>
-    <t>atap jpo kampus atma jaya le meridien akan copot</t>
-  </si>
-  <si>
-    <t>sukses program jokowi kampus bagi 2 000 beasiswa masyarakat</t>
-  </si>
-  <si>
-    <t>menag fachrul bangun kampus uiii depok mau selesai</t>
-  </si>
-  <si>
-    <t>nadiem jadi mendikbud jimly dunia kampus jangan rasa leceh</t>
-  </si>
-  <si>
-    <t>teten masduki tukang kritik kampus kini jadi menteri koperasi</t>
+    <t>demo hong kong picu sekolah tutup polisi tembak gas air mata kampu</t>
+  </si>
+  <si>
+    <t>sekolah kampus pusat belanja manila tutup sea games 2019</t>
+  </si>
+  <si>
+    <t>atap jpo kampus atma jaya le meridien copot</t>
+  </si>
+  <si>
+    <t>sukses program jokowi kampus 2 000 beasiswa masyarakat</t>
+  </si>
+  <si>
+    <t>menag fachrul bangun kampus uiii depok selesai</t>
+  </si>
+  <si>
+    <t>nadiem mendikbud jimly dunia kampus leceh</t>
+  </si>
+  <si>
+    <t>teten masduki tukang kritik kampus menteri koperasi</t>
   </si>
   <si>
     <t>sapi kak delapan kampus uin pekanbaru</t>
@@ -1972,10 +1972,10 @@
     <t>kemensos gandeng teliti kampus evaluasi program kub</t>
   </si>
   <si>
-    <t>kampus kairo jadi bahasa indonesia bahasa dua</t>
-  </si>
-  <si>
-    <t>tusuk wiranto sebut alumni usu jelas pihak kampu</t>
+    <t>kampus kairo bahasa indonesia bahasa</t>
+  </si>
+  <si>
+    <t>tusuk wiranto alumni usu kampu</t>
   </si>
   <si>
     <t>alas ugm batal acara ustaz abdul somad masjid kampu</t>
@@ -1984,19 +1984,19 @@
     <t>canda ujung maut 2 mahasiswa uin tenggelam embung kampu</t>
   </si>
   <si>
-    <t>sikap tegas kampus ipb henti dosen ab si buat bom molotov</t>
+    <t>sikap kampus ipb henti dosen ab si bom molotov</t>
   </si>
   <si>
     <t>tips cepat lulus barista kota daeng rajin kampus ngopi</t>
   </si>
   <si>
-    <t>mahasiswa asal papua ke kampu</t>
-  </si>
-  <si>
-    <t>menristekdikti sebut paham radikal ada kampu</t>
-  </si>
-  <si>
-    <t>menristekdikti fasilitas bebas dapat mahasiswa kampu</t>
+    <t>mahasiswa papua kampu</t>
+  </si>
+  <si>
+    <t>menristekdikti paham radikal kampu</t>
+  </si>
+  <si>
+    <t>menristekdikti fasilitas bebas mahasiswa kampu</t>
   </si>
   <si>
     <t>anti mainstream deret wisuda unik kampus itenas vir</t>
@@ -2005,25 +2005,25 @@
     <t>mahasiswa hong kong gelar aksi tolak ruu ekstradisi kampus taiwan</t>
   </si>
   <si>
-    <t>jumlah kampus surabaya izin mahasiswa demo</t>
+    <t>kampus surabaya izin mahasiswa demo</t>
   </si>
   <si>
     <t>1 anggota tni tewas pulang demonstran kampus uncen papua</t>
   </si>
   <si>
-    <t>geruduk mahasiswa universitas cendrawasih polri minta rektorat masuk kampu</t>
-  </si>
-  <si>
-    <t>universitas jember gagas kkn antar kampus sejawa timur</t>
+    <t>geruduk mahasiswa universitas cendrawasih polri rektorat masuk kampu</t>
+  </si>
+  <si>
+    <t>universitas jember gagas kkn kampus sejawa timur</t>
   </si>
   <si>
     <t>tolak lemah kpk puisi jokowi gema kampus biru ugm</t>
   </si>
   <si>
-    <t>aktris felicity huffman dienjara kait skandal suap masuk kampus elit</t>
-  </si>
-  <si>
-    <t>keren kampus hasil cipta bahan bakar baru karbondioksida</t>
+    <t>aktris felicity huffman dienjara kait skandal suap masuk kampus elite a</t>
+  </si>
+  <si>
+    <t>keren kampus hasil cipta bahan bakar karbondioksida</t>
   </si>
   <si>
     <t>kampus itb cirebon terjun balon pantau potensi gempa</t>
@@ -2032,7 +2032,7 @@
     <t>viral pelonco kampus ternate 4 pedoman ospek kemenristekdikti</t>
   </si>
   <si>
-    <t>ospek minum air ludah dpr minta kampus terus tingkat awa</t>
+    <t>ospek minum air ludah dpr kampus tingkat awa</t>
   </si>
   <si>
     <t>duga mesum lokasi kkn 2 mahasiswa samarinda panggil kampu</t>
@@ -2059,25 +2059,25 @@
     <t>berontak aliansi utara serang kampus militer myanmar 15 orang tewa</t>
   </si>
   <si>
-    <t>pilih rektor itb buka calon luar kampus daftar</t>
+    <t>pilih rektor itb buka calon kampus daftar</t>
   </si>
   <si>
     <t>putra sulung angelina jolie terima kampus gengsi korea selatan</t>
   </si>
   <si>
-    <t>raker luar kampus ikat alumni ui sekolah pascasarjana bahas 3 ini</t>
-  </si>
-  <si>
-    <t>jadi mahasiswa jadul bagaimana main film koboy kampus laku riset</t>
-  </si>
-  <si>
-    <t>kampus ung angkat bicara soal pungut rp50 juta mahasiswa baru</t>
-  </si>
-  <si>
-    <t>jerat ganja kampus ibu kota</t>
-  </si>
-  <si>
-    <t>siapa bandar pasok ganja puluh kilogram kampus jakarta</t>
+    <t>raker kampus ikat alumni ui sekolah pascasarjana bahas 3</t>
+  </si>
+  <si>
+    <t>mahasiswa jadul main film koboy kampus laku riset</t>
+  </si>
+  <si>
+    <t>kampus ung angkat bicara pungut rp50 juta mahasiswa</t>
+  </si>
+  <si>
+    <t>jerat ganja kampus kota</t>
+  </si>
+  <si>
+    <t>bandar pasok ganja puluh kilogram kampus jakarta</t>
   </si>
   <si>
     <t>duga sarang narkoba 6 kampus jakarta awas polisi</t>
@@ -2089,31 +2089,31 @@
     <t>kejut bintang film koboy kampus banjarmasin</t>
   </si>
   <si>
-    <t>80 kg ganja kering jadi sandungan 2 mahasiswa beprestasi kampus jakarta</t>
+    <t>80 kg ganja kering sandungan 2 mahasiswa beprestasi kampus jakarta</t>
   </si>
   <si>
     <t>polisi tangkap 2 mahasiswa edar ganja 80 kilogram kampus jakarta</t>
   </si>
   <si>
-    <t>kerja sama sea 5 kampus sedia beasiswa</t>
+    <t>kerja sea 5 kampus sedia beasiswa</t>
   </si>
   <si>
     <t>11 kg ganja temu ruang senat mahasiswa kampus jakarta timur</t>
   </si>
   <si>
-    <t>tum hmi sebut kampus jauh ormas antipancasila</t>
+    <t>tum hmi kampus ormas antipancasila</t>
   </si>
   <si>
     <t>suara vanesha prescilla alun album koboy kampu</t>
   </si>
   <si>
-    <t>gubernur riau larang warga bunyi terompet malam tahun baru</t>
-  </si>
-  <si>
-    <t>kabupaten siak riau jadi lokasi paling ideal lihat gerhana matahari cincin</t>
-  </si>
-  <si>
-    <t>bencana tanah gerak makin parah jalur lintas sumbar  riau ancam putu</t>
+    <t>gubernur riau larang warga bunyi terompet malam</t>
+  </si>
+  <si>
+    <t>kabupaten siak riau lokasi ideal lihat gerhana matahari cincin</t>
+  </si>
+  <si>
+    <t>bencana tanah gerak parah jalur lintas sumbar  riau ancam putu</t>
   </si>
   <si>
     <t>olivia zalianty dukung gera selamat lingkung hidup riau</t>
@@ -2125,19 +2125,19 @@
     <t>polisi riau sita ratus kardus rokok ilegal nila miliar rupiah</t>
   </si>
   <si>
-    <t>pemprov riau tetap status siaga darurat banjir longsor</t>
+    <t>pemprov riau status siaga darurat banjir longsor</t>
   </si>
   <si>
     <t>ditpolair riau gagal selundup ribu satwa lindung belangka</t>
   </si>
   <si>
-    <t>kaleidoskop 2019 tahun bencana kabut asap konflik satwa liar riau</t>
+    <t>kaleidoskop 2019 bencana kabut asap konflik satwa liar riau</t>
   </si>
   <si>
     <t>ekspor nonmigas pulau riau capai usd 6 73 miliar</t>
   </si>
   <si>
-    <t>selundup anak singa macan tutul hingga orang utan gagal polisi bksda riau</t>
+    <t>selundup anak singa macan tutul orang utan gagal polisi bksda riau</t>
   </si>
   <si>
     <t>akses jalan hubung antardesa riau putus akibat banjir</t>
@@ -2146,7 +2146,7 @@
     <t>polisi bksda riau gagal selundup satwa langka</t>
   </si>
   <si>
-    <t>prediksi kemarau panjang hantu riau 2020</t>
+    <t>prediksi kemarau hantu riau 2020</t>
   </si>
   <si>
     <t>banjir riau telan korban jiwa 2 balita tewas seret aru</t>
@@ -2158,7 +2158,7 @@
     <t>longsor jalan lintas sumbar  riau putu</t>
   </si>
   <si>
-    <t>duh 28 asn riau sandung kasus korupsi</t>
+    <t>duh 28 asn riau sandung korupsi</t>
   </si>
   <si>
     <t>klhk polri tangkap laku buru harimau sumatera riau</t>
@@ -2167,7 +2167,7 @@
     <t>bekuk buru riau polisi sita 4 ekor janin harimau topl</t>
   </si>
   <si>
-    <t>jelang pesta tahun baru polda riau tangkap 429 edar narkoba</t>
+    <t>jelang pesta polda riau tangkap 429 edar narkoba</t>
   </si>
   <si>
     <t>polda riau tembak bandar narkoba sindikat internasion</t>
@@ -2176,10 +2176,10 @@
     <t>3 harimau masuk kota pekanbaru terkam warga bbksda riau hoak</t>
   </si>
   <si>
-    <t>harimau mondarmandir mukim bbksda riau minta warga waspada</t>
-  </si>
-  <si>
-    <t>forum gajah sebut bunuh gajah riau aceh satu kelompok</t>
+    <t>harimau mondarmandir mukim bbksda riau warga waspada</t>
+  </si>
+  <si>
+    <t>forum gajah bunuh gajah riau aceh kelompok</t>
   </si>
   <si>
     <t>grasi eks gubernur riau annas maamun narasi lemah berantas korupsi</t>
@@ -2188,13 +2188,13 @@
     <t>alas jokowi ikan grasi eks gubernur riau annas maamun</t>
   </si>
   <si>
-    <t>jokowi beri grasi pidana korupsi eks gubernur riau annas maamun</t>
-  </si>
-  <si>
-    <t>hujan intensitas tinggi potensi landa daerah banjir riau</t>
-  </si>
-  <si>
-    <t>medco oleh dana bangun pltgu tenayan riau</t>
+    <t>jokowi grasi pidana korupsi eks gubernur riau annas maamun</t>
+  </si>
+  <si>
+    <t>hujan intensitas potensi landa daerah banjir riau</t>
+  </si>
+  <si>
+    <t>medco dana bangun pltgu tenayan riau</t>
   </si>
   <si>
     <t>modus curi minyak mentah usaha amerika riau libat mantan sekur</t>
@@ -2203,10 +2203,10 @@
     <t>buru gading gajah riau aksi rapi tinggal jejak</t>
   </si>
   <si>
-    <t>jadi korban buru gajah mati riau temu kondisi ena</t>
-  </si>
-  <si>
-    <t>terka sebab mati gajah temu busuk riau</t>
+    <t>korban buru gajah mati riau temu kondisi ena</t>
+  </si>
+  <si>
+    <t>terka mati gajah temu busuk riau</t>
   </si>
   <si>
     <t>nasib kapolres nama asep tugas singkat riau</t>
@@ -2215,85 +2215,85 @@
     <t>misteri bangkai gajah lahan konsesi pt arara abadi riau</t>
   </si>
   <si>
-    <t>aksi sama menghadang api karhutla riau</t>
-  </si>
-  <si>
-    <t>riau asal mula sebut bumi lancang kun</t>
-  </si>
-  <si>
-    <t>babak baru kasus kabut asap riau seret usaha sawit</t>
-  </si>
-  <si>
-    <t>densus 88 tembak satu duga teroris riau</t>
-  </si>
-  <si>
-    <t>polda riau ketat jaga usai bom polrestabes medan</t>
+    <t>aksi menghadang api karhutla riau</t>
+  </si>
+  <si>
+    <t>riau bumi lancang kun</t>
+  </si>
+  <si>
+    <t>babak kabut asap riau seret usaha sawit</t>
+  </si>
+  <si>
+    <t>densus 88 tembak duga teroris riau</t>
+  </si>
+  <si>
+    <t>polda riau ketat jaga bom polrestabes medan</t>
   </si>
   <si>
     <t>polisi tembak mati residivis narkoba jaring malaysia riau</t>
   </si>
   <si>
-    <t>ump 2020 riau tetap naik jadi rp 2 88 juta</t>
+    <t>ump 2020 riau rp 2 88 juta</t>
   </si>
   <si>
     <t>presiden pks target tang sembilan pilkada 2020 riau</t>
   </si>
   <si>
-    <t>mimpi stadion utama riau jadi tuan rumah piala dunia u20</t>
-  </si>
-  <si>
-    <t>soal konflik harimau manusia wwf riau relokasi bukan solusi</t>
-  </si>
-  <si>
-    <t>harimau masuk desa warga langir riau minta pemda turun tangan</t>
-  </si>
-  <si>
-    <t>3 orang tewas terkam harimau sumatera riau panjang 2019</t>
+    <t>mimpi stadion utama riau tuan rumah piala dunia u20</t>
+  </si>
+  <si>
+    <t>konflik harimau manusia wwf riau relokasi solusi</t>
+  </si>
+  <si>
+    <t>harimau masuk desa warga langir riau pemda turun tangan</t>
+  </si>
+  <si>
+    <t>3 orang tewas terkam harimau sumatera riau 2019</t>
   </si>
   <si>
     <t>harimau sumatera serang kerja bksda riau rumah</t>
   </si>
   <si>
-    <t>kronologi harimau sumatera terkam kerja hingga tewas riau</t>
-  </si>
-  <si>
-    <t>begini sistem kerja gardu induk pulau ngenang pulau riau</t>
-  </si>
-  <si>
-    <t>jaksa tinggi riau tahan sangka korupsi dana teliti didik</t>
+    <t>kronologi harimau sumatera terkam kerja tewas riau</t>
+  </si>
+  <si>
+    <t>sistem kerja gardu induk pulau ngenang pulau riau</t>
+  </si>
+  <si>
+    <t>jaksa riau tahan sangka korupsi dana teliti didik</t>
   </si>
   <si>
     <t>bbksda riau evakuasi ular piton kenyang kebun warga</t>
   </si>
   <si>
-    <t>atas karhutla gubernur riau lirik dashboard lancang kuning milik polda</t>
-  </si>
-  <si>
-    <t>indonesia tasbih sama ustadz abdul somad</t>
-  </si>
-  <si>
-    <t>harga baru kado tahun baru aki malam spesial tahun baru</t>
-  </si>
-  <si>
-    <t>sambut ganti tahun jumlah daerah apa kabar indonesia pagi</t>
+    <t>karhutla gubernur riau lirik dashboard lancang kuning milik polda</t>
+  </si>
+  <si>
+    <t>indonesia tasbih ustadz abdul somad</t>
+  </si>
+  <si>
+    <t>harga kado aki malam spesi</t>
+  </si>
+  <si>
+    <t>sambut ganti daerah kabar indonesia pagi</t>
   </si>
   <si>
     <t>jamin ketersediaanair bersih jokowi resmi bendung kamijoro bantul</t>
   </si>
   <si>
-    <t>banyak kasus cuat lama 2019 pasar modal bersih</t>
+    <t>cuat 2019 pasar modal bersih</t>
   </si>
   <si>
     <t>zina mamah dedeh</t>
   </si>
   <si>
-    <t>siap januari tarif tol cipali naik</t>
-  </si>
-  <si>
-    <t>prakira cuaca ganti tahun apa kabar indonesia pagi</t>
-  </si>
-  <si>
-    <t>perkosa ibu mati sidik jari</t>
+    <t>januari tarif tol cipali</t>
+  </si>
+  <si>
+    <t>prakira cuaca ganti kabar indonesia pagi</t>
+  </si>
+  <si>
+    <t>perkosa mati sidik jari</t>
   </si>
   <si>
     <t>wisata surfing indonesia indonesia plu</t>
@@ -2302,64 +2302,64 @@
     <t>one pride pro never quit 35 fight mot</t>
   </si>
   <si>
-    <t>kabar siang lokasi semarak akhir tahun</t>
+    <t>kabar siang lokasi semarak</t>
   </si>
   <si>
     <t>tim gegana aman tas curiga halaman masjid agung sunda kelapa</t>
   </si>
   <si>
-    <t>aman tahun baru polres boyolali kerah ratus personel gabung</t>
+    <t>aman polres boyolali kerah ratus personel gabung</t>
   </si>
   <si>
     <t>eklsklusif dialog tvone ahmad dhani beba</t>
   </si>
   <si>
-    <t>catat akhir tahun oneprix</t>
-  </si>
-  <si>
-    <t>jalur ganja tiga kota buru sergap</t>
+    <t>catat oneprix</t>
+  </si>
+  <si>
+    <t>jalur ganja kota buru sergap</t>
   </si>
   <si>
     <t>full kawin kontrak sisi gelap pariwisata puncak fakta</t>
   </si>
   <si>
-    <t>dendam balik serang novel aki malam</t>
-  </si>
-  <si>
-    <t>gunung anak krakatau erupsi keluar abu vulkanik setinggi 200 met</t>
-  </si>
-  <si>
-    <t>kunjung pasar johar presiden sama menteri gowes onthel bareng</t>
-  </si>
-  <si>
-    <t>deret artis jerat kasus prostitusi hingga narkoba catat akhir tahun 2019</t>
-  </si>
-  <si>
-    <t>stadion bumi wali mulai bebenah impi standar internasional sportone upd</t>
-  </si>
-  <si>
-    <t>libur akhir tahun arus lalu lintas puncak kawasan wisata bandung pantau padat</t>
-  </si>
-  <si>
-    <t>adab pengantin baru rumah mamah dedeh</t>
+    <t>dendam serang novel aki malam</t>
+  </si>
+  <si>
+    <t>gunung anak krakatau erupsi abu vulkanik 200 met</t>
+  </si>
+  <si>
+    <t>kunjung pasar johar presiden menteri gowes onthel bareng</t>
+  </si>
+  <si>
+    <t>deret artis jerat prostitusi narkoba catat 2019</t>
+  </si>
+  <si>
+    <t>stadion bumi wali bebenah impi standar internasional sportone upd</t>
+  </si>
+  <si>
+    <t>libur arus lintas puncak kawasan wisata bandung pantau padat</t>
+  </si>
+  <si>
+    <t>adab pengantin rumah mamah dedeh</t>
   </si>
   <si>
     <t>tembak usaha anak bupati tuntut ringan aki pagi</t>
   </si>
   <si>
-    <t>pssi rekrut shin tae yong jadi latih timnas senior sportone upd</t>
-  </si>
-  <si>
-    <t>inisiatif revisi uu kpk ujung kontroversi tiada henti catat akhir tahun 2019</t>
-  </si>
-  <si>
-    <t>bebas ahmad dhani akan film lama dalam penjara</t>
+    <t>pssi rekrut shin tae yong latih timnas senior sportone upd</t>
+  </si>
+  <si>
+    <t>inisiatif revisi uu kpk ujung kontroversi tiada henti catat 2019</t>
+  </si>
+  <si>
+    <t>bebas ahmad dhani film penjara</t>
   </si>
   <si>
     <t>full konferensi pers ahmad dhani beba</t>
   </si>
   <si>
-    <t>politis gerindra fadli zon sambut baik atas bebas ahmad dhani</t>
+    <t>politis gerindra fadli zon sambut bebas ahmad dhani</t>
   </si>
   <si>
     <t>ahmad dhani bebas massa jemput damping dhani pulang</t>
@@ -2368,16 +2368,16 @@
     <t>gibran gelar kompetisi esport hadiah ratus juta rupiah</t>
   </si>
   <si>
-    <t>kisruh aksi massa 22 mei 2019 catat akhir tahun 2019</t>
-  </si>
-  <si>
-    <t>panggung drama politik 2019 catat akhir tahun 2019</t>
+    <t>kisruh aksi massa 22 mei 2019 catat 2019</t>
+  </si>
+  <si>
+    <t>panggung drama politik 2019 catat 2019</t>
   </si>
   <si>
     <t>leon chandra mekanik handal racetech oneprix</t>
   </si>
   <si>
-    <t>dialog tvone gerindra umum cawagub dki apa tanggap pk</t>
+    <t>dialog tvone gerindra cawagub dki tanggap pk</t>
   </si>
   <si>
     <t>heboh wali murid tega tampar siswi sd makassar</t>
@@ -2386,13 +2386,13 @@
     <t>taqwa kuat bangsa martabat damai indonesia</t>
   </si>
   <si>
-    <t>shin tae yong sang latih baru timnas indonesia sportone mut</t>
-  </si>
-  <si>
-    <t>ugalugalan mobil seruduk pick logistik panggung tahun baru bundar hi</t>
-  </si>
-  <si>
-    <t>rafid topan sucipto expert bebek 4t 150 cc tune injection oneprix best rid</t>
+    <t>shin tae yong sang latih timnas indonesia sportone mut</t>
+  </si>
+  <si>
+    <t>ugalugalan mobil seruduk pick up logistik panggung bundar hi</t>
+  </si>
+  <si>
+    <t>rafid topan sucipto expert bebek 4t 150 cc tune up injection oneprix best rid</t>
   </si>
   <si>
     <t>best goal liga 2 2019 part 5 sporton</t>
@@ -2401,43 +2401,43 @@
     <t>niat mulia gagal laksana 60 korban tipu travel umroh bodong</t>
   </si>
   <si>
-    <t>modus jahat fintech abalabal apa kabar indonesia pagi</t>
+    <t>modus jahat fintech abalabal kabar indonesia pagi</t>
   </si>
   <si>
     <t>istri solehah rumah mamah dedeh</t>
   </si>
   <si>
-    <t>serang novel dalang wayang apa kabar indonesia malam</t>
-  </si>
-  <si>
-    <t>jokowiprabowo makin mesra hingga tak akur megawatipaloh catat akhir tahun 2019</t>
-  </si>
-  <si>
-    <t>jalan buntu tarik ulur rekonsiliasi mrt satu jokowiprabowo catat akhir tahun 2019</t>
-  </si>
-  <si>
-    <t>keras tarung politik panggung rebut kursi presiden catat akhir tahun 2019</t>
+    <t>serang novel dalang wayang kabar indonesia malam</t>
+  </si>
+  <si>
+    <t>jokowiprabowo mesra akur megawatipaloh catat 2019</t>
+  </si>
+  <si>
+    <t>jalan buntu tarik ulur rekonsiliasi mrt jokowiprabowo catat 2019</t>
+  </si>
+  <si>
+    <t>keras tarung politik panggung rebut kursi presiden catat 2019</t>
   </si>
   <si>
     <t>dialog tvone serang novel baswedan dendam</t>
   </si>
   <si>
-    <t>orang kendara ojol tinggal dunia usai timpa papan reklam</t>
-  </si>
-  <si>
-    <t>begini kondisi apotek senopati lagi tabrak mobil</t>
-  </si>
-  <si>
-    <t>muslim bagai satu tubuh damai indonesia</t>
-  </si>
-  <si>
-    <t>artis jerat narkoba nunung hingga zul zivilia catat akhir tahun 2019</t>
-  </si>
-  <si>
-    <t>cekcok masalah asmara pasang remaja nekat bakar diri</t>
-  </si>
-  <si>
-    <t>syamsul arifin expert bebek 4t 150 cc tune injection oneprix best rid</t>
+    <t>orang kendara ojol tinggal dunia timpa papan reklam</t>
+  </si>
+  <si>
+    <t>kondisi apotek senopati tabrak mobil</t>
+  </si>
+  <si>
+    <t>muslim tubuh damai indonesia</t>
+  </si>
+  <si>
+    <t>artis jerat narkoba nunung zul zivilia catat 2019</t>
+  </si>
+  <si>
+    <t>cekcok asmara pasang remaja nekat bakar</t>
+  </si>
+  <si>
+    <t>syamsul arifin expert bebek 4t 150 cc tune up injection oneprix best rid</t>
   </si>
   <si>
     <t>best goal liga 2 2019 part 4 sporton</t>
@@ -2446,40 +2446,40 @@
     <t>seru om way bareng betharia sonata etalk show tvon</t>
   </si>
   <si>
-    <t>pesona diva dian piesesha tak lekang masa etalk show</t>
-  </si>
-  <si>
-    <t>eksklusif serang novel baswedan tangkap apa kabar indonesia malam</t>
-  </si>
-  <si>
-    <t>heboh pbnu tagih kredit murah apa kabar indonesia malam</t>
+    <t>pesona diva dian piesesha lekang etalk show</t>
+  </si>
+  <si>
+    <t>eksklusif serang novel baswedan tangkap kabar indonesia malam</t>
+  </si>
+  <si>
+    <t>heboh pbnu tagih kredit murah kabar indonesia malam</t>
   </si>
   <si>
     <t>kabar sumut 27 desember 2019</t>
   </si>
   <si>
-    <t>soal uighur mahfud md sudah panggil dubes cina</t>
+    <t>uighur mahfud md panggil dubes cina</t>
   </si>
   <si>
     <t>best goal liga 2 2019 part 3 sporton</t>
   </si>
   <si>
-    <t>debat abdul chair ramadhan vs junimart girsang soal hukum jadi alat kuasa</t>
+    <t>debat abdul chair ramadhan vs junimart girsang hukum alat kuasa</t>
   </si>
   <si>
     <t>adu argumen rocky gerung vs junimart girsang kait demokrasi negara hukum</t>
   </si>
   <si>
-    <t>sebut nama habib rizieq shihab abdul chair ramadhan hukum jadi alat kuasa tinda</t>
-  </si>
-  <si>
-    <t>panas debat rocky gerung vs junimart girsang soal argumen jokowi tak paham pancasila</t>
-  </si>
-  <si>
-    <t>godfather jakarta john kei beba</t>
-  </si>
-  <si>
-    <t>mahfud md indonesia tak ikut campur soal uighur</t>
+    <t>nama habib rizieq shihab abdul chair ramadhan hukum alat kuasa tinda</t>
+  </si>
+  <si>
+    <t>panas debat rocky gerung vs junimart girsang argumen jokowi paham pancasila</t>
+  </si>
+  <si>
+    <t>godfather of jakarta john kei beba</t>
+  </si>
+  <si>
+    <t>mahfud md indonesia campur uighur</t>
   </si>
   <si>
     <t>aksi koboi lamborghini ujung bui</t>
@@ -2488,19 +2488,19 @@
     <t>raih syafaat sholawat assalamualaikum nusantara</t>
   </si>
   <si>
-    <t>libur panjang pantai kuta serbu wisatawan kabar siang lokasi</t>
+    <t>libur pantai kuta serbu wisatawan kabar siang lokasi</t>
   </si>
   <si>
     <t>kisah kampung kerang hijau jakarta utara liput khusu</t>
   </si>
   <si>
-    <t>warga barru sulawesi selatan geger temu benda mirip bom</t>
-  </si>
-  <si>
-    <t>libur akhir tahun antre panjang kendara padat pintu tol cikarang utama</t>
-  </si>
-  <si>
-    <t>milik lamborghini todong senpi apa kabar indonesia pagi</t>
+    <t>warga barru sulawesi selatan geger temu benda bom</t>
+  </si>
+  <si>
+    <t>libur antre kendara padat pintu tol cikarang utama</t>
+  </si>
+  <si>
+    <t>milik lamborghini todong senpi kabar indonesia pagi</t>
   </si>
   <si>
     <t>catat hukum demokrasi 2019</t>
@@ -2509,211 +2509,211 @@
     <t>catat hukum demokrasi 2019 sisi</t>
   </si>
   <si>
-    <t>debat abdul choir vs junimart soal world justice project</t>
+    <t>debat abdul choir vs junimart world justice project</t>
   </si>
   <si>
     <t>sambut gerhana matahari cincin karyawan tvone gelar sholat gerhana</t>
   </si>
   <si>
-    <t>junimart langgar ham lama belum tuntas diseleseikan cepat</t>
-  </si>
-  <si>
-    <t>akbar faizal hari parpol masalah 74 bupati gubernur produk oligarki</t>
-  </si>
-  <si>
-    <t>abdul tegak hukum indoesia jalan baik bahkan level rendah</t>
-  </si>
-  <si>
-    <t>debat rocky gerung vs junimart soal jokowi tak paham pancasila</t>
-  </si>
-  <si>
-    <t>warga baru sulawesi selatan geger temu benda mirip bom</t>
-  </si>
-  <si>
-    <t>ledak bom jadi panjang tahun 2019</t>
-  </si>
-  <si>
-    <t>kelam 2019 bagaimana nasib bisnis terbang 2020</t>
-  </si>
-  <si>
-    <t>tiga kasus polres tangsel ungkap lama 2019</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 5 peristiwa jadi kota bogor panjang tahun</t>
-  </si>
-  <si>
-    <t>257 kasus bakar medan panjang 2019 4 tinggal dunia</t>
-  </si>
-  <si>
-    <t>catat ikappi 201 pasar tradisional bakar panjang 2019 bas orang tewa</t>
-  </si>
-  <si>
-    <t>panjang 2019 74 kasus karhutla riau 81 laku tangkap</t>
-  </si>
-  <si>
-    <t>158 anggota polres jakbar naik pangkat hujung 2019</t>
+    <t>junimart langgar ham tuntas diseleseikan cepat</t>
+  </si>
+  <si>
+    <t>akbar faizal parpol 74 bupati gubernur produk oligarki</t>
+  </si>
+  <si>
+    <t>abdul tegak hukum indoesia jalan level rendah</t>
+  </si>
+  <si>
+    <t>debat rocky gerung vs junimart jokowi paham pancasila</t>
+  </si>
+  <si>
+    <t>warga sulawesi selatan geger temu benda bom</t>
+  </si>
+  <si>
+    <t>ledak bom 2019</t>
+  </si>
+  <si>
+    <t>kelam 2019 nasib bisnis terbang 2020</t>
+  </si>
+  <si>
+    <t>polres tangsel 2019</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 5 peristiwa kota bogor</t>
+  </si>
+  <si>
+    <t>257 bakar medan 2019 4 tinggal dunia</t>
+  </si>
+  <si>
+    <t>catat ikappi 201 pasar tradisional bakar 2019 bas orang tewa</t>
+  </si>
+  <si>
+    <t>2019 74 karhutla riau 81 laku tangkap</t>
+  </si>
+  <si>
+    <t>158 anggota polres jakbar pangkat hujung 2019</t>
   </si>
   <si>
     <t>kaleidoskop 2019 ka anjlok grobogan blora heboh warga</t>
   </si>
   <si>
-    <t>celaka tangsel tahun 2019 tingkat jelas polres tangsel</t>
-  </si>
-  <si>
-    <t>malam tahun baru 2020 tunjuk kembang api mall central park lebih banyak belum</t>
-  </si>
-  <si>
-    <t>kasus kriminal jakarta timur turun 2019</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 demo besar bagai negara</t>
-  </si>
-  <si>
-    <t>taman jinja hingga negeri atas awan 4 tempat wisata viral 2019</t>
-  </si>
-  <si>
-    <t>kaleidoskop didik 15 smp baik nasional versi un 2019</t>
-  </si>
-  <si>
-    <t>akhir tahun 2019 unjung taman margasatwa ragunan turun</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 jalan liku anies lawan bisnis hibur malam awal jabat saat</t>
-  </si>
-  <si>
-    <t>sebab bmw motorrad tarik ikut motogp</t>
-  </si>
-  <si>
-    <t>kilas didik 15 smp negeri baik indonesia panjang 2019</t>
-  </si>
-  <si>
-    <t>polisi sebut kasus narkoba turun 12 03 persen banding 2018</t>
+    <t>celaka tangsel 2019 tingkat polres tangsel</t>
+  </si>
+  <si>
+    <t>malam 2020 kembang api mall central park</t>
+  </si>
+  <si>
+    <t>kriminal jakarta timur turun 2019</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 demo negara</t>
+  </si>
+  <si>
+    <t>taman jinja negeri awan 4 wisata viral 2019</t>
+  </si>
+  <si>
+    <t>kaleidoskop didik 15 smp nasional versi un 2019</t>
+  </si>
+  <si>
+    <t>2019 unjung taman margasatwa ragunan turun</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 jalan liku anies lawan bisnis hibur malam jabat</t>
+  </si>
+  <si>
+    <t>bmw motorrad tarik motogp</t>
+  </si>
+  <si>
+    <t>kilas didik 15 smp negeri indonesia 2019</t>
+  </si>
+  <si>
+    <t>polisi narkoba turun 12 03 persen banding 2018</t>
   </si>
   <si>
     <t>kaleidoskop 2019 cabor olahraga indonesia impresif sea gam</t>
   </si>
   <si>
-    <t>naik edar uang tembus rp 6 072 triliun november 2019</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 indonesia punya 1 decacorn 4 unicorn</t>
-  </si>
-  <si>
-    <t>tahun baru 2020 perlu resolusi</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 tipu daya tipu ibu kota kasus djeni hingga rumah syariah</t>
-  </si>
-  <si>
-    <t>10 miliarder paling dermawan panjang 2019</t>
+    <t>edar uang tembus rp 6 072 triliun november 2019</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 indonesia 1 decacorn 4 unicorn</t>
+  </si>
+  <si>
+    <t>2020 resolusi</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 tipu daya tipu kota djeni rumah syariah</t>
+  </si>
+  <si>
+    <t>10 miliarder dermawan 2019</t>
   </si>
   <si>
     <t>persib bandung rencana bangun sport cent</t>
   </si>
   <si>
-    <t>200 pidana mati eksekusi 2019 jelas jagung</t>
-  </si>
-  <si>
-    <t>ridwan kamil siap rp 4 1 miliar raih medali sea gam</t>
+    <t>200 pidana mati eksekusi 2019 jagung</t>
+  </si>
+  <si>
+    <t>ridwan kamil rp 4 1 miliar raih medali sea gam</t>
   </si>
   <si>
     <t>kaleidoskop motogp 2019 marquez juara lorenzo pensiun quartararo</t>
   </si>
   <si>
-    <t>7 nikah artis indonesia curi perhati panjang 2019</t>
-  </si>
-  <si>
-    <t>25 lagu kpop baik panjang 2019 versi billboard</t>
+    <t>7 nikah artis indonesia curi perhati 2019</t>
+  </si>
+  <si>
+    <t>25 lagu kpop 2019 versi billboard</t>
   </si>
   <si>
     <t>populer internasional mayat kapal hantu jepang 5 aksi teror 2019</t>
   </si>
   <si>
-    <t>populer nasional tahun marah jokowi pks percaya quick count</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 wajah baru jakarta makin modern</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 liga inggris sinar redup leicester hingga muncul var</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 jalan kasus prada dp laku mutilasi kasih hingga vonis umur hidup</t>
+    <t>populer nasional marah jokowi pks percaya quick count</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 wajah jakarta modern</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 liga inggris sinar redup leicester muncul var</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 jalan prada dp laku mutilasi kasih vonis umur hidup</t>
   </si>
   <si>
     <t>populer kompasiana blokir situs ilegal natal safari anies hingarbingar</t>
   </si>
   <si>
-    <t>kaleidoskop 2019 kisruh ormas minta jatah parkir beka</t>
-  </si>
-  <si>
-    <t>kevin de bruyne jadi raja assist liga inggris akhir tahun 2019</t>
-  </si>
-  <si>
-    <t>jaksa agung beri sanksi 174 jaksa panjang 2019</t>
-  </si>
-  <si>
-    <t>panjang 2019 sumut bangun 89 kilometer jalan 169 meter jembatan</t>
-  </si>
-  <si>
-    <t>kaleidoskop 5 aksi teror jadi dunia panjang 2019</t>
-  </si>
-  <si>
-    <t>polres jakarta barat ringkus 304 preman panjang 2019</t>
-  </si>
-  <si>
-    <t>675 celaka lalu lintas jadi kota bekas panjang 2019</t>
-  </si>
-  <si>
-    <t>panjang 2019 jadi 54 kasus cabul sumedang</t>
+    <t>kaleidoskop 2019 kisruh ormas jatah parkir beka</t>
+  </si>
+  <si>
+    <t>kevin de bruyne raja assist liga inggris 2019</t>
+  </si>
+  <si>
+    <t>jaksa agung sanksi 174 jaksa 2019</t>
+  </si>
+  <si>
+    <t>2019 sumut bangun 89 kilometer jalan 169 meter jembatan</t>
+  </si>
+  <si>
+    <t>kaleidoskop 5 aksi teror dunia 2019</t>
+  </si>
+  <si>
+    <t>polres jakarta barat ringkus 304 preman 2019</t>
+  </si>
+  <si>
+    <t>675 celaka lintas kota bekas 2019</t>
+  </si>
+  <si>
+    <t>2019 54 cabul sumedang</t>
   </si>
   <si>
     <t>10 396 lamar lolos administrasi cpns bpk informasi lengkap</t>
   </si>
   <si>
-    <t>jaksa agung satu bulan 10 hukum mati perkara narkoba</t>
-  </si>
-  <si>
-    <t>jumlah guna transjakarta capai 800 ribu per hari 2019</t>
-  </si>
-  <si>
-    <t>angka celaka lalu lintas 2019 tingkat</t>
-  </si>
-  <si>
-    <t>panjang 2019 jampidum paling banyak tangan perkara narkotika</t>
-  </si>
-  <si>
-    <t>bal united pasti main senior tahan liga 1 2020</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 jumlah ruas tol alami naik tarif</t>
-  </si>
-  <si>
-    <t>jahat turun 2019 persentasi ungkap kasus tingkat</t>
+    <t>jaksa agung 10 hukum mati perkara narkoba</t>
+  </si>
+  <si>
+    <t>transjakarta capai 800 ribu 2019</t>
+  </si>
+  <si>
+    <t>angka celaka lintas 2019 tingkat</t>
+  </si>
+  <si>
+    <t>2019 jampidum tangan perkara narkotika</t>
+  </si>
+  <si>
+    <t>bal united main senior tahan liga 1 2020</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 ruas tol alami tarif</t>
+  </si>
+  <si>
+    <t>jahat turun 2019 persentasi tingkat</t>
   </si>
   <si>
     <t>kaleidoskop 2019 ratus tugas selenggara milu jabar gugur</t>
   </si>
   <si>
-    <t>13 bencana besar jadi panjang 2019</t>
+    <t>13 bencana 2019</t>
   </si>
   <si>
     <t>pres 82 2019 atur tugas fungsi ditjen budaya</t>
   </si>
   <si>
-    <t>5 film indonesia laris panjang tahun 2019</t>
-  </si>
-  <si>
-    <t>catat 41 bunuh massal panjang 2019 banyak sejak 1970an</t>
-  </si>
-  <si>
-    <t>2019 bnpb catat jadi 3 768 bencana indonesia</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 usai asai bagaimana nasib freeport ini</t>
-  </si>
-  <si>
-    <t>kuliah ui cek dulu peluang masuk snmptn 2019</t>
+    <t>5 film indonesia laris 2019</t>
+  </si>
+  <si>
+    <t>as catat 41 bunuh massal 2019 1970an</t>
+  </si>
+  <si>
+    <t>2019 bnpb catat 3 768 bencana indonesia</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 asai nasib freeport</t>
+  </si>
+  <si>
+    <t>kuliah ui cek peluang masuk snmptn 2019</t>
   </si>
   <si>
     <t>daftar 10 main mahal liga 1 2019 marko simic nomor</t>
@@ -2722,94 +2722,94 @@
     <t>30 desember 2019 taman margasatwa ragunan tutup libur satwa</t>
   </si>
   <si>
-    <t>tahun 2019 jadi bukti tingkat diri universitas islam indonesia</t>
-  </si>
-  <si>
-    <t>sela tak mau sentuh zona degradasi liga 1</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 rusuh papua buntut kasus rasial hoak</t>
+    <t>2019 bukti tingkat universitas islam indonesia</t>
+  </si>
+  <si>
+    <t>sentuh zona degradasi liga 1</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 rusuh papua buntut rasial hoak</t>
   </si>
   <si>
     <t>kaleidoskop 2019 jakarta serba instagrammable era anies baswedan</t>
   </si>
   <si>
-    <t>kaleidoskop 2019 6 tentang jokowi libat makar hingga ujung jeruji besi</t>
+    <t>kaleidoskop 2019 6 jokowi libat makar ujung jeruji besi</t>
   </si>
   <si>
     <t>kaleidoskop 2019 serang hoaks hantam kpu</t>
   </si>
   <si>
-    <t>urus jumlah tonton 2019 persija nomor satu seasia tenggara</t>
-  </si>
-  <si>
-    <t>kalah messi cr7 main baik 2019 versi dubai globe soccer award</t>
-  </si>
-  <si>
-    <t>rengkuh menang raksasa steven gerrard akhir 2019 cara indah</t>
-  </si>
-  <si>
-    <t>tutup 2019 menteri basuki tinjau empat proyek infrastruktur</t>
-  </si>
-  <si>
-    <t>catat icw 2019 tahun hancur kpk sponsor presiden dpr</t>
-  </si>
-  <si>
-    <t>kbs minta maaf usai henti tampil apink gayo daechukje 2019</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 kasus korupsi jerat bupati hingga kepala dinas eks residen pati</t>
-  </si>
-  <si>
-    <t>sedih tampil potong kbs gayo daechukje 2019 apink minta laku adil</t>
-  </si>
-  <si>
-    <t>kaleidoskop 2019 bongkar kasus mayat karung hingga juru parkir bakar hidup</t>
-  </si>
-  <si>
-    <t>persib juara liga 1 putri 2019 sejarah baru ukir</t>
+    <t>urus tonton 2019 persija nomor seasia tenggara</t>
+  </si>
+  <si>
+    <t>kalah messi cr7 main 2019 versi dubai globe soccer award</t>
+  </si>
+  <si>
+    <t>rengkuh menang raksasa steven gerrard 2019 indah</t>
+  </si>
+  <si>
+    <t>tutup 2019 menteri basuki tinjau proyek infrastruktur</t>
+  </si>
+  <si>
+    <t>catat icw 2019 hancur kpk sponsor presiden dpr</t>
+  </si>
+  <si>
+    <t>kbs maaf henti tampil apink gayo daechukje 2019</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 korupsi jerat bupati kepala dinas eks residen pati</t>
+  </si>
+  <si>
+    <t>sedih tampil potong kbs gayo daechukje 2019 apink laku adil</t>
+  </si>
+  <si>
+    <t>kaleidoskop 2019 bongkar mayat karung juru parkir bakar hidup</t>
+  </si>
+  <si>
+    <t>persib juara liga 1 putri 2019 sejarah ukir</t>
   </si>
   <si>
     <t>bal united baya wakil indonesia asean club championship</t>
   </si>
   <si>
-    <t>sang latih ungkap kunci sukses persib juara liga 1 putri 2019</t>
+    <t>sang latih kunci sukses persib juara liga 1 putri 2019</t>
   </si>
   <si>
     <t>halsey harga khusus organisasi tunawisma</t>
   </si>
   <si>
-    <t>kpk terima hasil vonis 4 tahun eddy sindoro</t>
-  </si>
-  <si>
-    <t>anies sebut lepas saham bir tak perlu kaji</t>
-  </si>
-  <si>
-    <t>lima besar box office korea pekan</t>
-  </si>
-  <si>
-    <t>imbang barito sela empat final piala presiden</t>
-  </si>
-  <si>
-    <t>bawel jin cengiran abu whole new world aladdin</t>
+    <t>kpk terima hasil vonis 4 eddy sindoro</t>
+  </si>
+  <si>
+    <t>anies lepas saham bir kaji</t>
+  </si>
+  <si>
+    <t>box office korea pekan</t>
+  </si>
+  <si>
+    <t>imbang barito final piala presiden</t>
+  </si>
+  <si>
+    <t>bawel jin cengiran abu a whole new world aladdin</t>
   </si>
   <si>
     <t>hikayat congyang minum idola sungkan puja</t>
   </si>
   <si>
-    <t>imigrasi timika deportasi 12 tambang asal china korsel</t>
+    <t>imigrasi timika deportasi 12 tambang china korsel</t>
   </si>
   <si>
     <t>polisi periksa intensif pria bawa magasin mako brimob diy</t>
   </si>
   <si>
-    <t>lipi buka soal reorganisasi isu jual buku loak</t>
-  </si>
-  <si>
-    <t>juventus vs atletico ronaldo tahu bakal hattrick</t>
-  </si>
-  <si>
-    <t>video ketua kpk serah tanggung jawab kpk presiden</t>
+    <t>lipi buka reorganisasi isu jual buku loak</t>
+  </si>
+  <si>
+    <t>juventus vs atletico ronaldo hattrick</t>
+  </si>
+  <si>
+    <t>video ketua kpk serah tanggung kpk presiden</t>
   </si>
   <si>
     <t>yeonjun tari latar dancer utama txt</t>
@@ -2827,31 +2827,31 @@
     <t>brg bantah tuding sumur bor fiktif kalteng</t>
   </si>
   <si>
-    <t>genjot investasi tak cukup rombak 72 undang</t>
-  </si>
-  <si>
-    <t>hakim sebut aspri menpora buat sepakat koni</t>
-  </si>
-  <si>
-    <t>video saksi 01 sebut jokowi hadir latih tot tkn</t>
-  </si>
-  <si>
-    <t>ruf tentara keluar jalur kembali sumpah prajurit</t>
-  </si>
-  <si>
-    <t>kpk aku irjen firli pernah langgar etik</t>
-  </si>
-  <si>
-    <t>cukup bawa proposal warga gelar acara setu babakan</t>
-  </si>
-  <si>
-    <t>8 agenda akhir pekan minggu</t>
+    <t>genjot investasi rombak 72 undang</t>
+  </si>
+  <si>
+    <t>hakim aspri menpora sepakat koni</t>
+  </si>
+  <si>
+    <t>video saksi 01 jokowi hadir latih tot tkn</t>
+  </si>
+  <si>
+    <t>ma ruf tentara jalur sumpah prajurit</t>
+  </si>
+  <si>
+    <t>kpk irjen firli langgar etik</t>
+  </si>
+  <si>
+    <t>bawa proposal warga gelar acara setu babakan</t>
+  </si>
+  <si>
+    <t>8 agenda pekan minggu</t>
   </si>
   <si>
     <t>kpk periksa romi kait duga suap dak tasikmalaya</t>
   </si>
   <si>
-    <t>rahmat baequni minta maaf soal ceramah kpps tewas racun</t>
+    <t>rahmat baequni maaf ceramah kpps tewas racun</t>
   </si>
   <si>
     <t>enzim usus ubah golong darah manusia</t>
@@ -2863,34 +2863,34 @@
     <t>video wisata tepi sungai pyongyang</t>
   </si>
   <si>
-    <t>deputi tindak kpk firli tunjuk jadi kapolda sumsel</t>
+    <t>deputi tindak kpk firli kapolda sumsel</t>
   </si>
   <si>
     <t>syarat paul pogba gabung juventu</t>
   </si>
   <si>
-    <t>ketua kpk sebut polri butuh irjen firli</t>
-  </si>
-  <si>
-    <t>video hakim cecar soal kpu cepat kesah hasil pilpr</t>
-  </si>
-  <si>
-    <t>sela vs persija akhir imbang</t>
+    <t>ketua kpk polri butuh irjen firli</t>
+  </si>
+  <si>
+    <t>video hakim cecar kpu cepat kesah hasil pilpr</t>
+  </si>
+  <si>
+    <t>vs persija imbang</t>
   </si>
   <si>
     <t>timnas brasil bantah intai peru pakai dron</t>
   </si>
   <si>
-    <t>de ligt sebut terima rayu ronaldo juventu</t>
-  </si>
-  <si>
-    <t>video chile menang susah payah atas ekuador copa america</t>
-  </si>
-  <si>
-    <t>hasil copa america 2019 chile menang 21 atas ekuador</t>
-  </si>
-  <si>
-    <t>chile vs ekuador imbang 11 babak pertama copa america</t>
+    <t>de ligt terima rayu ronaldo juventu</t>
+  </si>
+  <si>
+    <t>video chile menang susah payah ekuador copa america</t>
+  </si>
+  <si>
+    <t>hasil copa america 2019 chile menang 21 ekuador</t>
+  </si>
+  <si>
+    <t>chile vs ekuador imbang 11 babak copa america</t>
   </si>
   <si>
     <t>suap dak kpk usut peran romi wali kota tasikmalaya</t>
@@ -2902,7 +2902,7 @@
     <t>video baca apel persada presiden joko widodo</t>
   </si>
   <si>
-    <t>rest area sumber macet jadi titik temu mudik</t>
+    <t>rest area sumber macet titik temu mudik</t>
   </si>
   <si>
     <t>video momen sby keluarga lepas pergi ani yudhoyono</t>
@@ -2911,43 +2911,43 @@
     <t>video exo tunggu exol hut 18 transmedia</t>
   </si>
   <si>
-    <t>video nanti nct dream tampil hut 18 transmedia</t>
-  </si>
-  <si>
-    <t>james bond gabung film cinderella versi baru</t>
-  </si>
-  <si>
-    <t>jadi gumiho lee dongwook adu akting sama jo boah</t>
+    <t>video nct dream tampil hut 18 transmedia</t>
+  </si>
+  <si>
+    <t>james bond gabung film cinderella versi</t>
+  </si>
+  <si>
+    <t>gumiho lee dongwook adu akting jo boah</t>
   </si>
   <si>
     <t>anthony ginting semifinal bwf world tour fin</t>
   </si>
   <si>
-    <t>sunat hukum eks bupati buton suap akil mochtar</t>
+    <t>ma sunat hukum eks bupati buton suap akil mochtar</t>
   </si>
   <si>
     <t>ahsan hendra gagal sempurna grup b bwf world tour fin</t>
   </si>
   <si>
-    <t>7 cara baik lebat rambut bayi</t>
-  </si>
-  <si>
-    <t>daftar klub lolos 32 besar liga europa</t>
-  </si>
-  <si>
-    <t>kapolri menko polhukam temu tak bahas kasus novel</t>
+    <t>7 lebat rambut bayi</t>
+  </si>
+  <si>
+    <t>daftar klub lolos 32 liga europa</t>
+  </si>
+  <si>
+    <t>kapolri menko polhukam temu bahas novel</t>
   </si>
   <si>
     <t>bwf world tour finals marcus kevin kalah endo watanab</t>
   </si>
   <si>
-    <t>suap meikarta eks bos lippo cikarang sebut jebak anak buah</t>
+    <t>suap meikarta eks bos lippo cikarang jebak anak buah</t>
   </si>
   <si>
     <t>posisi mil ganti torino liga europa</t>
   </si>
   <si>
-    <t>bank dunia kucur pinjam rp3 5 madrasah ri</t>
+    <t>bank dunia kucur pinjam rp3 5 t madrasah ri</t>
   </si>
   <si>
     <t>jokowi teken pres jabat fungsional tni</t>
@@ -2962,40 +2962,40 @@
     <t>video bupati pacitan bentuk tim darurat hepat</t>
   </si>
   <si>
-    <t>jadwal empat final copa america venezuela vs argentina</t>
-  </si>
-  <si>
-    <t>video pasien hepatitis pacitan tambah jadi 824 orang</t>
-  </si>
-  <si>
-    <t>5 momen penting brasil lolos semifinal copa america</t>
-  </si>
-  <si>
-    <t>derita sakit kuning pacitan terus tambah</t>
+    <t>jadwal final copa america venezuela vs argentina</t>
+  </si>
+  <si>
+    <t>video pasien hepatitis a pacitan 824 orang</t>
+  </si>
+  <si>
+    <t>5 momen brasil lolos semifinal copa america</t>
+  </si>
+  <si>
+    <t>derita sakit kuning pacitan</t>
   </si>
   <si>
     <t>politikus pdip pimpin komisi iv v dpr</t>
   </si>
   <si>
-    <t>politikus pdip pimpin banggar dpr ibas jadi wakil</t>
+    <t>politikus pdip pimpin banggar dpr ibas wakil</t>
   </si>
   <si>
     <t>8 makan super sehat ginj</t>
   </si>
   <si>
-    <t>video sering macet lalu lintas kawasan kemang rekayasa</t>
+    <t>video macet lintas kawasan kemang rekayasa</t>
   </si>
   <si>
     <t>video bawa senjata demo kendari 6 polisi sanksi</t>
   </si>
   <si>
-    <t>video iur bpjs sehat resmi naik tahun depan</t>
-  </si>
-  <si>
-    <t>video menkes awan bentuk tim atas masalah bpj</t>
-  </si>
-  <si>
-    <t>video hujan buat atas krisis air bandung</t>
+    <t>video iur bpjs sehat resmi</t>
+  </si>
+  <si>
+    <t>video menkes awan bentuk tim bpj</t>
+  </si>
+  <si>
+    <t>video hujan krisis air bandung</t>
   </si>
   <si>
     <t>video delegasi dunia melayu dunia islam indonesia</t>
@@ -3004,31 +3004,31 @@
     <t>video tawur manggarai pecah 1 polisi luka bacok</t>
   </si>
   <si>
-    <t>video kang sora soal film baru rendang bajaj</t>
-  </si>
-  <si>
-    <t>harga saham bjbr naik 1 18 persen jadi rp1 715</t>
-  </si>
-  <si>
-    <t>eni saragih penuh panggil kpk jadi saksi samin tan</t>
-  </si>
-  <si>
-    <t>anggota dprd bengkal mangkir panggil kpk soal suap</t>
-  </si>
-  <si>
-    <t>eks sekretaris aju praperadilan kpk siap hadap</t>
+    <t>video kang sora film rendang bajaj</t>
+  </si>
+  <si>
+    <t>harga saham bjbr 1 18 persen rp1 715</t>
+  </si>
+  <si>
+    <t>eni saragih penuh panggil kpk saksi samin tan</t>
+  </si>
+  <si>
+    <t>anggota dprd bengkal mangkir panggil kpk suap</t>
+  </si>
+  <si>
+    <t>eks sekretaris ma aju praperadilan kpk hadap</t>
   </si>
   <si>
     <t>valeinalum sepakat tunda penandatanganan divestasi saham</t>
   </si>
   <si>
-    <t>banjir bandang labura satu keluarga hilang temu</t>
-  </si>
-  <si>
-    <t>lagu baru hailee steinfeld duga niall horan</t>
-  </si>
-  <si>
-    <t>impor bawang politikus pdip dakwa terima suap rp3 5</t>
+    <t>banjir bandang labura keluarga hilang temu</t>
+  </si>
+  <si>
+    <t>lagu hailee steinfeld duga niall horan</t>
+  </si>
+  <si>
+    <t>impor bawang politikus pdip dakwa terima suap rp3 5 m</t>
   </si>
   <si>
     <t>kpk rampung sidi eks dirut ptpn iii</t>
@@ -3040,7 +3040,7 @@
     <t>ronaldo bikin heboh netizen man bun</t>
   </si>
   <si>
-    <t>video daftar atlet baik 2019</t>
+    <t>video daftar atlet 2019</t>
   </si>
   <si>
     <t>video daftar atlet buruk 2019</t>
@@ -3049,19 +3049,19 @@
     <t>daftar film buku 2019 favorit barack obama</t>
   </si>
   <si>
-    <t>bupati indramayu nonaktif supendi duga terima suap rp3 6</t>
+    <t>bupati indramayu nonaktif supendi duga terima suap rp3 6 m</t>
   </si>
   <si>
     <t>huawei bangun jaring bas sdn semen indonesia</t>
   </si>
   <si>
-    <t>program kemenperin bangun masa depan bangsa</t>
+    <t>program kemenperin bangun bangsa</t>
   </si>
   <si>
     <t>bph migas inspeksi bbm maumer</t>
   </si>
   <si>
-    <t>buka mata pikir lewat konser 1975 jakarta</t>
+    <t>buka mata pikir konser the 1975 jakarta</t>
   </si>
   <si>
     <t>kapolri pimpin sertijab kapolda papua riau sultra</t>
@@ -3070,7 +3070,7 @@
     <t>stabil politik negeri topang ihsg pekan</t>
   </si>
   <si>
-    <t>tagar giampaolo gema usai mil kalah fiorentina</t>
+    <t>tagar giampaolo out gema mil kalah fiorentina</t>
   </si>
   <si>
     <t>hasil liga italia 10 main mil kalah fiorentina</t>
@@ -3079,22 +3079,22 @@
     <t>kpk jeblos eks jabat kemenpora lapas tangerang</t>
   </si>
   <si>
-    <t>amnesty ulas kasus novel baswedan kongr</t>
-  </si>
-  <si>
-    <t>praperadilan kivlan ahli jelas proses tetap sangka</t>
-  </si>
-  <si>
-    <t>bupati nonaktif remigo vonis 7 tahun keluarga maki kpk</t>
-  </si>
-  <si>
-    <t>amnesty bahas kasus novel baswedan kongres malam</t>
-  </si>
-  <si>
-    <t>jelang lawan timnas indonesia u16 vietnam aku stabil</t>
-  </si>
-  <si>
-    <t>anies minta waspada kredit macet rumah dp 0 rupiah</t>
+    <t>amnesty ulas novel baswedan kongres a</t>
+  </si>
+  <si>
+    <t>praperadilan kivlan ahli proses sangka</t>
+  </si>
+  <si>
+    <t>bupati nonaktif remigo vonis 7 keluarga maki kpk</t>
+  </si>
+  <si>
+    <t>amnesty bahas novel baswedan kongres as malam</t>
+  </si>
+  <si>
+    <t>jelang lawan timnas indonesia u16 vietnam stabil</t>
+  </si>
+  <si>
+    <t>anies waspada kredit macet rumah dp 0 rupiah</t>
   </si>
   <si>
     <t>video polisi tangkap pasok narkoba nunung</t>
@@ -3106,10 +3106,10 @@
     <t>klasemen piala aff u15 timnas indonesia gagal puncak</t>
   </si>
   <si>
-    <t>timnas indonesia u15 tahan timor leste bima tetap pua</t>
-  </si>
-  <si>
-    <t>sekda jabar eks bos lippo cikarang cegah luar negeri</t>
+    <t>timnas indonesia u15 tahan timor leste bima pua</t>
+  </si>
+  <si>
+    <t>sekda jabar eks bos lippo cikarang cegah negeri</t>
   </si>
 </sst>
 </file>

</xml_diff>